<commit_message>
fix file header / names... added spectral type
</commit_message>
<xml_diff>
--- a/results/removed_rows.xlsx
+++ b/results/removed_rows.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,20 +444,22 @@
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="21" customWidth="1" min="12" max="12"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
-    <col width="15" customWidth="1" min="14" max="14"/>
-    <col width="8" customWidth="1" min="15" max="15"/>
-    <col width="9" customWidth="1" min="16" max="16"/>
-    <col width="21" customWidth="1" min="17" max="17"/>
-    <col width="22" customWidth="1" min="18" max="18"/>
+    <col width="21" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="9" customWidth="1" min="17" max="17"/>
+    <col width="21" customWidth="1" min="18" max="18"/>
     <col width="22" customWidth="1" min="19" max="19"/>
-    <col width="7" customWidth="1" min="20" max="20"/>
-    <col width="14" customWidth="1" min="21" max="21"/>
+    <col width="22" customWidth="1" min="20" max="20"/>
+    <col width="7" customWidth="1" min="21" max="21"/>
     <col width="14" customWidth="1" min="22" max="22"/>
-    <col width="16" customWidth="1" min="23" max="23"/>
-    <col width="15" customWidth="1" min="24" max="24"/>
-    <col width="18" customWidth="1" min="25" max="25"/>
+    <col width="14" customWidth="1" min="23" max="23"/>
+    <col width="16" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="18" customWidth="1" min="26" max="26"/>
+    <col width="24" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -518,72 +520,82 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>spectraltype_esphs_dr2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>dr2_source_id</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>dr3_source_id</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>source_id_dr3</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ra_dr3</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>dec_dr3</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>phot_g_mean_mag_dr3</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>phot_bp_mean_mag_dr3</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>phot_rp_mean_mag_dr3</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>bp_rp</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>parallax_dr3</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>teff_gspphot</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>mass_flame_dr3</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>lum_flame_dr3</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>radius_flame_dr3</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>spectraltype_esphs_dr3</t>
         </is>
       </c>
     </row>
@@ -625,10 +637,15 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>1462061709995883136</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>1462061709996744448</t>
         </is>
@@ -669,10 +686,15 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>1586968533015434624</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>1586968533013974528</t>
         </is>
@@ -705,12 +727,12 @@
       <c r="H4" t="n">
         <v>5143.4501953125</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>2595463996992115840</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>2595463996992115840</t>
         </is>
@@ -745,10 +767,15 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>2974726131970829952</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>2974726136265625088</t>
         </is>
@@ -789,10 +816,15 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>3213958769587525888</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>3213958769589070848</t>
         </is>
@@ -827,10 +859,15 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
           <t>3234412606443085824</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>3234412602147418496</t>
         </is>
@@ -874,10 +911,15 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>3575733210781078016</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>3575733210778695808</t>
         </is>
@@ -921,10 +963,15 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
           <t>3943232534138172672</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>3943232534137347072</t>
         </is>
@@ -957,12 +1004,12 @@
       <c r="H10" t="n">
         <v>5095.63330078125</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>5426587107149861120</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>5426587107149861120</t>
         </is>
@@ -997,10 +1044,15 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
           <t>598180818531935232</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>598180818531355776</t>
         </is>
@@ -1033,12 +1085,12 @@
       <c r="H12" t="n">
         <v>6022</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>6719152945029845376</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>6719152945032456832</t>
         </is>
@@ -1071,12 +1123,12 @@
       <c r="H13" t="n">
         <v>5190.33349609375</v>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>6719152945032456832</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>6719152945032456832</t>
         </is>
@@ -1111,10 +1163,15 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>776067089642433664</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>776067093937332992</t>
         </is>

</xml_diff>

<commit_message>
new SQL implementation in progress; Also testing calculate_rv_precision
</commit_message>
<xml_diff>
--- a/results/removed_rows.xlsx
+++ b/results/removed_rows.xlsx
@@ -442,7 +442,7 @@
     <col width="19" customWidth="1" min="7" max="7"/>
     <col width="19" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="21" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="24" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
@@ -654,49 +654,38 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1586968533015434624</t>
+          <t>2043885295912608512</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>225.2329125375929</v>
+        <v>284.2576611101138</v>
       </c>
       <c r="C3" t="n">
-        <v>45.42768754176895</v>
+        <v>32.90073932392183</v>
       </c>
       <c r="D3" t="n">
-        <v>8.464728355407715</v>
+        <v>5.116928577423096</v>
       </c>
       <c r="E3" t="n">
-        <v>9.400127410888672</v>
+        <v>5.428450107574463</v>
       </c>
       <c r="F3" t="n">
-        <v>7.524870872497559</v>
+        <v>4.655242443084717</v>
       </c>
       <c r="G3" t="n">
-        <v>85.37534836100293</v>
+        <v>66.5742243900887</v>
       </c>
       <c r="H3" t="n">
-        <v>4256.30322265625</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.07281243801116943</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.6930326223373413</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
+        <v>5932</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1586968533015434624</t>
+          <t>2043885295912608512</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1586968533013974528</t>
+          <t>2043885295914530944</t>
         </is>
       </c>
     </row>
@@ -980,152 +969,152 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>4590758227640885248</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>142.6740032632142</v>
+        <v>271.7561269586085</v>
       </c>
       <c r="C10" t="n">
-        <v>-40.466567086598</v>
+        <v>30.56233941836619</v>
       </c>
       <c r="D10" t="n">
-        <v>4.803853511810303</v>
+        <v>4.892927646636963</v>
       </c>
       <c r="E10" t="n">
-        <v>3.975138902664185</v>
+        <v>5.211727142333984</v>
       </c>
       <c r="F10" t="n">
-        <v>3.240525007247925</v>
+        <v>4.491597652435303</v>
       </c>
       <c r="G10" t="n">
-        <v>54.30532208415497</v>
+        <v>63.53576695184549</v>
       </c>
       <c r="H10" t="n">
-        <v>5095.63330078125</v>
+        <v>6009</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>4590758227640885248</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>4590758227637479040</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>598180818531935232</t>
+          <t>5426587107149861120</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>130.6865172420918</v>
+        <v>142.6740032632142</v>
       </c>
       <c r="C11" t="n">
-        <v>9.5539723965289</v>
+        <v>-40.466567086598</v>
       </c>
       <c r="D11" t="n">
-        <v>8.946824073791504</v>
+        <v>4.803853511810303</v>
       </c>
       <c r="E11" t="n">
-        <v>9.887347221374512</v>
+        <v>3.975138902664185</v>
       </c>
       <c r="F11" t="n">
-        <v>7.971009254455566</v>
+        <v>3.240525007247925</v>
       </c>
       <c r="G11" t="n">
-        <v>64.3680016469628</v>
+        <v>54.30532208415497</v>
       </c>
       <c r="H11" t="n">
-        <v>3873</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
+        <v>5095.63330078125</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>598180818531935232</t>
+          <t>5426587107149861120</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>598180818531355776</t>
+          <t>5426587107149861120</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6719152945029845376</t>
+          <t>598180818531935232</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>286.6054157588619</v>
+        <v>130.6865172420918</v>
       </c>
       <c r="C12" t="n">
-        <v>-37.06488085942344</v>
+        <v>9.5539723965289</v>
       </c>
       <c r="D12" t="n">
-        <v>4.717123985290527</v>
+        <v>8.946824073791504</v>
       </c>
       <c r="E12" t="n">
-        <v>4.816995620727539</v>
+        <v>9.887347221374512</v>
       </c>
       <c r="F12" t="n">
-        <v>4.114394664764404</v>
+        <v>7.971009254455566</v>
       </c>
       <c r="G12" t="n">
-        <v>57.85828017971518</v>
+        <v>64.3680016469628</v>
       </c>
       <c r="H12" t="n">
-        <v>6022</v>
+        <v>3873</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>6719152945029845376</t>
+          <t>598180818531935232</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>6719152945032456832</t>
+          <t>598180818531355776</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6719152945032456832</t>
+          <t>6719152945029845376</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>286.6053079615535</v>
+        <v>286.6054157588619</v>
       </c>
       <c r="C13" t="n">
-        <v>-37.06450354954132</v>
+        <v>-37.06488085942344</v>
       </c>
       <c r="D13" t="n">
-        <v>4.760257244110107</v>
+        <v>4.717123985290527</v>
       </c>
       <c r="E13" t="n">
-        <v>4.791435241699219</v>
+        <v>4.816995620727539</v>
       </c>
       <c r="F13" t="n">
-        <v>3.94169807434082</v>
+        <v>4.114394664764404</v>
       </c>
       <c r="G13" t="n">
-        <v>58.69555998807621</v>
+        <v>57.85828017971518</v>
       </c>
       <c r="H13" t="n">
-        <v>5190.33349609375</v>
+        <v>6022</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>6719152945032456832</t>
+          <t>6719152945029845376</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1137,43 +1126,38 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>776067089642433664</t>
+          <t>6719152945032456832</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>161.3393177357646</v>
+        <v>286.6053079615535</v>
       </c>
       <c r="C14" t="n">
-        <v>38.51241559503183</v>
+        <v>-37.06450354954132</v>
       </c>
       <c r="D14" t="n">
-        <v>8.667779922485352</v>
+        <v>4.760257244110107</v>
       </c>
       <c r="E14" t="n">
-        <v>9.488222122192383</v>
+        <v>4.791435241699219</v>
       </c>
       <c r="F14" t="n">
-        <v>7.58256721496582</v>
+        <v>3.94169807434082</v>
       </c>
       <c r="G14" t="n">
-        <v>72.98709001875206</v>
+        <v>58.69555998807621</v>
       </c>
       <c r="H14" t="n">
-        <v>4100</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
+        <v>5190.33349609375</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>776067089642433664</t>
+          <t>6719152945032456832</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>776067093937332992</t>
+          <t>6719152945032456832</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
optimise Older wroking version
</commit_message>
<xml_diff>
--- a/results/removed_rows.xlsx
+++ b/results/removed_rows.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,21 +440,21 @@
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
     <col width="19" customWidth="1" min="7" max="7"/>
-    <col width="19" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="11" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
     <col width="24" customWidth="1" min="12" max="12"/>
     <col width="21" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
-    <col width="15" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
-    <col width="9" customWidth="1" min="17" max="17"/>
+    <col width="21" customWidth="1" min="15" max="15"/>
+    <col width="19" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
     <col width="21" customWidth="1" min="18" max="18"/>
     <col width="22" customWidth="1" min="19" max="19"/>
     <col width="22" customWidth="1" min="20" max="20"/>
-    <col width="7" customWidth="1" min="21" max="21"/>
-    <col width="14" customWidth="1" min="22" max="22"/>
+    <col width="19" customWidth="1" min="21" max="21"/>
+    <col width="19" customWidth="1" min="22" max="22"/>
     <col width="14" customWidth="1" min="23" max="23"/>
     <col width="16" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
@@ -623,17 +623,25 @@
       <c r="G2" t="n">
         <v>55.12479618884052</v>
       </c>
-      <c r="H2" t="n">
-        <v>4109</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.6421307921409607</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.107005387544632</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.7143532633781433</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>3905.417</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.6421308</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.10700539</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.71435326</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -654,301 +662,325 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2043885295912608512</t>
+          <t>1552921051659352960</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>284.2576611101138</v>
+        <v>199.941227089661</v>
       </c>
       <c r="C3" t="n">
-        <v>32.90073932392183</v>
+        <v>47.77792679548974</v>
       </c>
       <c r="D3" t="n">
-        <v>5.116928577423096</v>
+        <v>7.948930263519287</v>
       </c>
       <c r="E3" t="n">
-        <v>5.428450107574463</v>
+        <v>8.774880409240723</v>
       </c>
       <c r="F3" t="n">
-        <v>4.655242443084717</v>
+        <v>6.670772075653076</v>
       </c>
       <c r="G3" t="n">
-        <v>66.5742243900887</v>
-      </c>
-      <c r="H3" t="n">
-        <v>5932</v>
+        <v>109.9837414044669</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4051.515</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.06580374</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.52064663</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2043885295912608512</t>
+          <t>1552921051659352960</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2043885295914530944</t>
+          <t>1552921055949679616</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2595463996992115840</t>
+          <t>1586968533015434624</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>336.6440634509766</v>
+        <v>225.2329125375929</v>
       </c>
       <c r="C4" t="n">
-        <v>-16.74185644464832</v>
+        <v>45.42768754176895</v>
       </c>
       <c r="D4" t="n">
-        <v>6.198555946350098</v>
+        <v>8.464728355407715</v>
       </c>
       <c r="E4" t="n">
-        <v>6.208871841430664</v>
+        <v>9.400127410888672</v>
       </c>
       <c r="F4" t="n">
-        <v>5.265100002288818</v>
+        <v>7.524870872497559</v>
       </c>
       <c r="G4" t="n">
-        <v>51.50789426625737</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5143.4501953125</v>
+        <v>85.37534836100293</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3601.6807</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.07281244</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.6930326</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2595463996992115840</t>
+          <t>1586968533015434624</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2595463996992115840</t>
+          <t>1586968533013974528</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2974726131970829952</t>
+          <t>2043885295908064128</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>75.61785590280779</v>
+        <v>284.2572876496914</v>
       </c>
       <c r="C5" t="n">
-        <v>-21.25784077680808</v>
+        <v>32.90057478653039</v>
       </c>
       <c r="D5" t="n">
-        <v>7.750740051269531</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8.57557487487793</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6.656546115875244</v>
+        <v>7.467142105102539</v>
       </c>
       <c r="G5" t="n">
-        <v>119.3398737310191</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4063.596435546875</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
+        <v>67.78145508350882</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2974726131970829952</t>
+          <t>2043885295908064128</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2974726136265625088</t>
+          <t>2043885295914530944</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3213958769587525888</t>
+          <t>2043885295912608512</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>79.80577003837008</v>
+        <v>284.2576611101138</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.073222913358394</v>
+        <v>32.90073932392183</v>
       </c>
       <c r="D6" t="n">
-        <v>7.478399753570557</v>
+        <v>5.116928577423096</v>
       </c>
       <c r="E6" t="n">
-        <v>8.042928695678711</v>
+        <v>5.428450107574463</v>
       </c>
       <c r="F6" t="n">
-        <v>6.742774486541748</v>
+        <v>4.655242443084717</v>
       </c>
       <c r="G6" t="n">
-        <v>63.65137588808516</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4976</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.2233356088399887</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.748258650302887</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>K</t>
+        <v>66.5742243900887</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>5932.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1.4960319</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1.1580325</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>3213958769587525888</t>
+          <t>2043885295912608512</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>3213958769589070848</t>
+          <t>2043885295914530944</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3234412606443085824</t>
+          <t>2595463996992115840</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>80.65646942221296</v>
+        <v>336.6440634509766</v>
       </c>
       <c r="C7" t="n">
-        <v>2.602451244119687</v>
+        <v>-16.74185644464832</v>
       </c>
       <c r="D7" t="n">
-        <v>7.53508996963501</v>
+        <v>6.198555946350098</v>
       </c>
       <c r="E7" t="n">
-        <v>8.008501052856445</v>
+        <v>6.208871841430664</v>
       </c>
       <c r="F7" t="n">
-        <v>6.799147129058838</v>
+        <v>5.265100002288818</v>
       </c>
       <c r="G7" t="n">
-        <v>50.39430355852318</v>
-      </c>
-      <c r="H7" t="n">
-        <v>4837</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>K</t>
+        <v>51.50789426625737</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>5143.45</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>3234412606443085824</t>
+          <t>2595463996992115840</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>3234412602147418496</t>
+          <t>2595463996992115840</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3575733210781078016</t>
+          <t>2974726131970829952</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>180.1856175191175</v>
+        <v>75.61785590280779</v>
       </c>
       <c r="C8" t="n">
-        <v>-10.44820514671702</v>
+        <v>-21.25784077680808</v>
       </c>
       <c r="D8" t="n">
-        <v>5.328901290893555</v>
+        <v>7.750740051269531</v>
       </c>
       <c r="E8" t="n">
-        <v>5.751168727874756</v>
+        <v>8.57557487487793</v>
       </c>
       <c r="F8" t="n">
-        <v>4.824667453765869</v>
+        <v>6.656546115875244</v>
       </c>
       <c r="G8" t="n">
-        <v>78.75648094040741</v>
-      </c>
-      <c r="H8" t="n">
-        <v>5518.5</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.8779153823852539</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.8789317011833191</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1.028767466545105</v>
+        <v>119.3398737310191</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>4063.5964</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.06656814</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.52055275</t>
+        </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>K</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>3575733210781078016</t>
+          <t>2974726131970829952</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>3575733210778695808</t>
+          <t>2974726136265625088</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3943232534138172672</t>
+          <t>3213958769587525888</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>196.5638957330539</v>
+        <v>79.80577003837008</v>
       </c>
       <c r="C9" t="n">
-        <v>20.72965678223564</v>
+        <v>-3.073222913358394</v>
       </c>
       <c r="D9" t="n">
-        <v>8.969438552856445</v>
+        <v>7.478399753570557</v>
       </c>
       <c r="E9" t="n">
-        <v>9.729983329772949</v>
+        <v>8.042928695678711</v>
       </c>
       <c r="F9" t="n">
-        <v>8.007077217102051</v>
+        <v>6.742774486541748</v>
       </c>
       <c r="G9" t="n">
-        <v>50.90347875548716</v>
-      </c>
-      <c r="H9" t="n">
-        <v>4122.9033203125</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.6415486335754395</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.10798329859972</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.6824297308921814</v>
+        <v>63.65137588808516</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4587.147</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.22333561</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.74825865</t>
+        </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -957,117 +989,178 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>3943232534138172672</t>
+          <t>3213958769587525888</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>3943232534137347072</t>
+          <t>3213958769589070848</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4590758227640885248</t>
+          <t>3234412606443085824</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>271.7561269586085</v>
+        <v>80.65646942221296</v>
       </c>
       <c r="C10" t="n">
-        <v>30.56233941836619</v>
+        <v>2.602451244119687</v>
       </c>
       <c r="D10" t="n">
-        <v>4.892927646636963</v>
+        <v>7.53508996963501</v>
       </c>
       <c r="E10" t="n">
-        <v>5.211727142333984</v>
+        <v>8.008501052856445</v>
       </c>
       <c r="F10" t="n">
-        <v>4.491597652435303</v>
+        <v>6.799147129058838</v>
       </c>
       <c r="G10" t="n">
-        <v>63.53576695184549</v>
-      </c>
-      <c r="H10" t="n">
-        <v>6009</v>
+        <v>50.39430355852318</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>4837.0</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.803856</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.287645</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.6787785</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>4590758227640885248</t>
+          <t>3234412606443085824</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>4590758227637479040</t>
+          <t>3234412602147418496</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>3575733210781078016</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>142.6740032632142</v>
+        <v>180.1856175191175</v>
       </c>
       <c r="C11" t="n">
-        <v>-40.466567086598</v>
+        <v>-10.44820514671702</v>
       </c>
       <c r="D11" t="n">
-        <v>4.803853511810303</v>
+        <v>5.328901290893555</v>
       </c>
       <c r="E11" t="n">
-        <v>3.975138902664185</v>
+        <v>5.751168727874756</v>
       </c>
       <c r="F11" t="n">
-        <v>3.240525007247925</v>
+        <v>4.824667453765869</v>
       </c>
       <c r="G11" t="n">
-        <v>54.30532208415497</v>
-      </c>
-      <c r="H11" t="n">
-        <v>5095.63330078125</v>
+        <v>78.75648094040741</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>5510.1235</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.8837685</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.859334</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1.0129887</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>3575733210781078016</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>3575733210778695808</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>598180818531935232</t>
+          <t>3943232534138172672</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>130.6865172420918</v>
+        <v>196.5638957330539</v>
       </c>
       <c r="C12" t="n">
-        <v>9.5539723965289</v>
+        <v>20.72965678223564</v>
       </c>
       <c r="D12" t="n">
-        <v>8.946824073791504</v>
+        <v>8.969438552856445</v>
       </c>
       <c r="E12" t="n">
-        <v>9.887347221374512</v>
+        <v>9.729983329772949</v>
       </c>
       <c r="F12" t="n">
-        <v>7.971009254455566</v>
+        <v>8.007077217102051</v>
       </c>
       <c r="G12" t="n">
-        <v>64.3680016469628</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3873</v>
+        <v>50.90347875548716</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>4006.3718</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.64154863</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.1079833</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.68242973</t>
+        </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1076,88 +1169,507 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>598180818531935232</t>
+          <t>3943232534138172672</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>598180818531355776</t>
+          <t>3943232534137347072</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6719152945029845376</t>
+          <t>4590758227637479040</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>286.6054157588619</v>
+        <v>271.7558821637892</v>
       </c>
       <c r="C13" t="n">
-        <v>-37.06488085942344</v>
+        <v>30.56263953176465</v>
       </c>
       <c r="D13" t="n">
-        <v>4.717123985290527</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4.816995620727539</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4.114394664764404</v>
+        <v>8.130936622619629</v>
       </c>
       <c r="G13" t="n">
-        <v>57.85828017971518</v>
-      </c>
-      <c r="H13" t="n">
-        <v>6022</v>
+        <v>53.97691200055367</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>6719152945029845376</t>
+          <t>4590758227637479040</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>6719152945032456832</t>
+          <t>4590758227637479040</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>4590758227640885248</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>271.7561269586085</v>
+      </c>
+      <c r="C14" t="n">
+        <v>30.56233941836619</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4.892927646636963</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.211727142333984</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4.491597652435303</v>
+      </c>
+      <c r="G14" t="n">
+        <v>63.53576695184549</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>6009.0</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2.0126045</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1.3089633</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>4590758227640885248</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>4590758227637479040</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5426587107149861120</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>142.6740032632142</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-40.466567086598</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.803853511810303</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.975138902664185</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3.240525007247925</v>
+      </c>
+      <c r="G15" t="n">
+        <v>54.30532208415497</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>5095.6333</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>5426587107149861120</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>5426587107149861120</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>5853498713160606720</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>217.3934657426036</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-62.67618210292382</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8.953612327575684</v>
+      </c>
+      <c r="E16" t="n">
+        <v>11.38292598724365</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7.586430072784424</v>
+      </c>
+      <c r="G16" t="n">
+        <v>768.5003653333918</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>3295.5</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>5853498713160606720</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>5853498713190524032</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5853498713160606720</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>217.3934657426036</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-62.67618210292382</v>
+      </c>
+      <c r="D17" t="n">
+        <v>8.953612327575684</v>
+      </c>
+      <c r="E17" t="n">
+        <v>11.38292598724365</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7.586430072784424</v>
+      </c>
+      <c r="G17" t="n">
+        <v>768.5003653333918</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>3295.5</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>5853498713160606720</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>5853498713190525696</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>5853498713190525696</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>217.3923214720088</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-62.67607511676666</v>
+      </c>
+      <c r="R17" t="n">
+        <v>8.984748840332031</v>
+      </c>
+      <c r="S17" t="n">
+        <v>11.37311553955078</v>
+      </c>
+      <c r="T17" t="n">
+        <v>7.568535327911377</v>
+      </c>
+      <c r="U17" t="n">
+        <v>3.804580211639404</v>
+      </c>
+      <c r="V17" t="n">
+        <v>768.0665391873573</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>2829.3542</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>0.0015221541</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>0.16237111</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>598180818531935232</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>130.6865172420918</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9.5539723965289</v>
+      </c>
+      <c r="D18" t="n">
+        <v>8.946824073791504</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9.887347221374512</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7.971009254455566</v>
+      </c>
+      <c r="G18" t="n">
+        <v>64.3680016469628</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>3873.0</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.3356494</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1.2673832</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>598180818531935232</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>598180818531355776</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>6719152945029845376</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>286.6054157588619</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-37.06488085942344</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4.717123985290527</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.816995620727539</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4.114394664764404</v>
+      </c>
+      <c r="G19" t="n">
+        <v>57.85828017971518</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>6022.0</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2.852196</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1.5515323</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>6719152945029845376</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
           <t>6719152945032456832</t>
         </is>
       </c>
-      <c r="B14" t="n">
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>6719152945032456832</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>286.6053079615535</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C20" t="n">
         <v>-37.06450354954132</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D20" t="n">
         <v>4.760257244110107</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E20" t="n">
         <v>4.791435241699219</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F20" t="n">
         <v>3.94169807434082</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G20" t="n">
         <v>58.69555998807621</v>
       </c>
-      <c r="H14" t="n">
-        <v>5190.33349609375</v>
-      </c>
-      <c r="M14" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>5190.3335</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>6719152945032456832</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>6719152945032456832</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>756853643637996160</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>169.543435666958</v>
+      </c>
+      <c r="C21" t="n">
+        <v>31.5264998339419</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4.594314098358154</v>
+      </c>
+      <c r="E21" t="n">
+        <v>7.022503852844238</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3.809747219085693</v>
+      </c>
+      <c r="G21" t="n">
+        <v>114.4866699181447</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>3821.5</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>1.5513859</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2.8414814</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>756853643637996160</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>756853643638639104</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>776067089642433664</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>161.3393177357646</v>
+      </c>
+      <c r="C22" t="n">
+        <v>38.51241559503183</v>
+      </c>
+      <c r="D22" t="n">
+        <v>8.667779922485352</v>
+      </c>
+      <c r="E22" t="n">
+        <v>9.488222122192383</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7.58256721496582</v>
+      </c>
+      <c r="G22" t="n">
+        <v>72.98709001875206</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>4100.0</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.07476281</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.5419107</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>776067089642433664</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>776067093937332992</t>
         </is>
       </c>
     </row>

</xml_diff>